<commit_message>
Analysis of saltation heights
</commit_message>
<xml_diff>
--- a/Metadata/GrainSizeMetadata.xlsx
+++ b/Metadata/GrainSizeMetadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="13820" yWindow="0" windowWidth="25600" windowHeight="14240" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SurfaceSamples" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1315" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1318" uniqueCount="32">
   <si>
     <t>Filename</t>
   </si>
@@ -369,8 +369,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="177">
+  <cellStyleXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -604,7 +608,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="177">
+  <cellStyles count="181">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -693,6 +697,8 @@
     <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -781,6 +787,8 @@
     <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4908,10 +4916,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H220"/>
+  <dimension ref="A1:H221"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="A121" sqref="A121"/>
+      <selection activeCell="E122" sqref="E122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6657,7 +6665,7 @@
     </row>
     <row r="67" spans="1:8">
       <c r="A67" s="36" t="str">
-        <f t="shared" ref="A67:A129" si="1">B67&amp;"_"&amp;TEXT(C67,"yyyy-mm-dd")&amp;"_BSNE_"&amp;D67&amp;"_"&amp;TEXT(E67,"HHMM")&amp;"_"&amp;TEXT(F67,"HHMM")</f>
+        <f t="shared" ref="A67:A130" si="1">B67&amp;"_"&amp;TEXT(C67,"yyyy-mm-dd")&amp;"_BSNE_"&amp;D67&amp;"_"&amp;TEXT(E67,"HHMM")&amp;"_"&amp;TEXT(F67,"HHMM")</f>
         <v>Oceano_2015-05-19_BSNE_B2_1413_1513</v>
       </c>
       <c r="B67" s="42" t="s">
@@ -8089,7 +8097,7 @@
     <row r="122" spans="1:8">
       <c r="A122" s="36" t="str">
         <f t="shared" si="1"/>
-        <v>Oceano_2015-05-27_BSNE_A4_1618_1748</v>
+        <v>Oceano_2015-05-27_BSNE_A4_1408_1608</v>
       </c>
       <c r="B122" s="42" t="s">
         <v>5</v>
@@ -8101,10 +8109,10 @@
         <v>15</v>
       </c>
       <c r="E122" s="41">
-        <v>0.6791666666666667</v>
+        <v>0.58888888888888891</v>
       </c>
       <c r="F122" s="41">
-        <v>0.7416666666666667</v>
+        <v>0.67222222222222217</v>
       </c>
       <c r="G122" s="37"/>
       <c r="H122" s="40" t="s">
@@ -8114,7 +8122,7 @@
     <row r="123" spans="1:8">
       <c r="A123" s="36" t="str">
         <f t="shared" si="1"/>
-        <v>Oceano_2015-05-27_BSNE_B1_1408_1608</v>
+        <v>Oceano_2015-05-27_BSNE_A4_1618_1748</v>
       </c>
       <c r="B123" s="42" t="s">
         <v>5</v>
@@ -8123,13 +8131,13 @@
         <v>42151</v>
       </c>
       <c r="D123" s="42" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E123" s="41">
-        <v>0.58888888888888891</v>
+        <v>0.6791666666666667</v>
       </c>
       <c r="F123" s="41">
-        <v>0.67222222222222217</v>
+        <v>0.7416666666666667</v>
       </c>
       <c r="G123" s="37"/>
       <c r="H123" s="40" t="s">
@@ -8139,7 +8147,7 @@
     <row r="124" spans="1:8">
       <c r="A124" s="36" t="str">
         <f t="shared" si="1"/>
-        <v>Oceano_2015-05-27_BSNE_B1_1618_1748</v>
+        <v>Oceano_2015-05-27_BSNE_B1_1408_1608</v>
       </c>
       <c r="B124" s="42" t="s">
         <v>5</v>
@@ -8151,10 +8159,10 @@
         <v>9</v>
       </c>
       <c r="E124" s="41">
-        <v>0.6791666666666667</v>
+        <v>0.58888888888888891</v>
       </c>
       <c r="F124" s="41">
-        <v>0.7416666666666667</v>
+        <v>0.67222222222222217</v>
       </c>
       <c r="G124" s="37"/>
       <c r="H124" s="40" t="s">
@@ -8164,7 +8172,7 @@
     <row r="125" spans="1:8">
       <c r="A125" s="36" t="str">
         <f t="shared" si="1"/>
-        <v>Oceano_2015-05-27_BSNE_B2_1408_1608</v>
+        <v>Oceano_2015-05-27_BSNE_B1_1618_1748</v>
       </c>
       <c r="B125" s="42" t="s">
         <v>5</v>
@@ -8173,13 +8181,13 @@
         <v>42151</v>
       </c>
       <c r="D125" s="42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E125" s="41">
-        <v>0.58888888888888891</v>
+        <v>0.6791666666666667</v>
       </c>
       <c r="F125" s="41">
-        <v>0.67222222222222217</v>
+        <v>0.7416666666666667</v>
       </c>
       <c r="G125" s="37"/>
       <c r="H125" s="40" t="s">
@@ -8189,7 +8197,7 @@
     <row r="126" spans="1:8">
       <c r="A126" s="36" t="str">
         <f t="shared" si="1"/>
-        <v>Oceano_2015-05-27_BSNE_B2_1618_1748</v>
+        <v>Oceano_2015-05-27_BSNE_B2_1408_1608</v>
       </c>
       <c r="B126" s="42" t="s">
         <v>5</v>
@@ -8201,10 +8209,10 @@
         <v>10</v>
       </c>
       <c r="E126" s="41">
-        <v>0.6791666666666667</v>
+        <v>0.58888888888888891</v>
       </c>
       <c r="F126" s="41">
-        <v>0.7416666666666667</v>
+        <v>0.67222222222222217</v>
       </c>
       <c r="G126" s="37"/>
       <c r="H126" s="40" t="s">
@@ -8214,7 +8222,7 @@
     <row r="127" spans="1:8">
       <c r="A127" s="36" t="str">
         <f t="shared" si="1"/>
-        <v>Oceano_2015-05-27_BSNE_B4_1408_1608</v>
+        <v>Oceano_2015-05-27_BSNE_B2_1618_1748</v>
       </c>
       <c r="B127" s="42" t="s">
         <v>5</v>
@@ -8223,13 +8231,13 @@
         <v>42151</v>
       </c>
       <c r="D127" s="42" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E127" s="41">
-        <v>0.58888888888888891</v>
+        <v>0.6791666666666667</v>
       </c>
       <c r="F127" s="41">
-        <v>0.67222222222222217</v>
+        <v>0.7416666666666667</v>
       </c>
       <c r="G127" s="37"/>
       <c r="H127" s="40" t="s">
@@ -8237,213 +8245,211 @@
       </c>
     </row>
     <row r="128" spans="1:8">
-      <c r="A128" s="44" t="str">
+      <c r="A128" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v>Oceano_2015-05-27_BSNE_B4_1408_1608</v>
+      </c>
+      <c r="B128" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C128" s="38">
+        <v>42151</v>
+      </c>
+      <c r="D128" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="E128" s="41">
+        <v>0.58888888888888891</v>
+      </c>
+      <c r="F128" s="41">
+        <v>0.67222222222222217</v>
+      </c>
+      <c r="G128" s="37"/>
+      <c r="H128" s="40" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8">
+      <c r="A129" s="44" t="str">
         <f t="shared" si="1"/>
         <v>Oceano_2015-05-27_BSNE_B4_1618_1748</v>
       </c>
-      <c r="B128" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="C128" s="46">
+      <c r="B129" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C129" s="46">
         <v>42151</v>
       </c>
-      <c r="D128" s="45" t="s">
+      <c r="D129" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="E128" s="47">
+      <c r="E129" s="47">
         <v>0.6791666666666667</v>
       </c>
-      <c r="F128" s="47">
+      <c r="F129" s="47">
         <v>0.7416666666666667</v>
       </c>
-      <c r="G128" s="48"/>
-      <c r="H128" s="49" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8">
-      <c r="A129" s="31" t="str">
+      <c r="G129" s="48"/>
+      <c r="H129" s="49" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8">
+      <c r="A130" s="31" t="str">
         <f t="shared" si="1"/>
         <v>Oceano_2015-05-28_BSNE_A3_1149_1712</v>
       </c>
-      <c r="B129" s="52" t="s">
-        <v>5</v>
-      </c>
-      <c r="C129" s="33">
+      <c r="B130" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C130" s="33">
         <v>42152</v>
       </c>
-      <c r="D129" s="52" t="s">
+      <c r="D130" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="E129" s="51">
+      <c r="E130" s="51">
         <v>0.49236111111111108</v>
       </c>
-      <c r="F129" s="51">
+      <c r="F130" s="51">
         <v>0.71666666666666667</v>
       </c>
-      <c r="G129" s="32"/>
-      <c r="H129" s="35" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8">
-      <c r="A130" s="44" t="str">
-        <f t="shared" ref="A130:A193" si="3">B130&amp;"_"&amp;TEXT(C130,"yyyy-mm-dd")&amp;"_BSNE_"&amp;D130&amp;"_"&amp;TEXT(E130,"HHMM")&amp;"_"&amp;TEXT(F130,"HHMM")</f>
+      <c r="G130" s="32"/>
+      <c r="H130" s="35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8">
+      <c r="A131" s="44" t="str">
+        <f t="shared" ref="A131:A194" si="3">B131&amp;"_"&amp;TEXT(C131,"yyyy-mm-dd")&amp;"_BSNE_"&amp;D131&amp;"_"&amp;TEXT(E131,"HHMM")&amp;"_"&amp;TEXT(F131,"HHMM")</f>
         <v>Oceano_2015-05-28_BSNE_A4_1149_1712</v>
       </c>
-      <c r="B130" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="C130" s="46">
+      <c r="B131" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C131" s="46">
         <v>42152</v>
       </c>
-      <c r="D130" s="45" t="s">
+      <c r="D131" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="E130" s="47">
+      <c r="E131" s="47">
         <v>0.49236111111111108</v>
       </c>
-      <c r="F130" s="47">
+      <c r="F131" s="47">
         <v>0.71666666666666667</v>
       </c>
-      <c r="G130" s="48"/>
-      <c r="H130" s="49" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8">
-      <c r="A131" s="31" t="str">
+      <c r="G131" s="48"/>
+      <c r="H131" s="49" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8">
+      <c r="A132" s="31" t="str">
         <f t="shared" si="3"/>
         <v>Oceano_2015-06-01_BSNE_A3_1033_1500</v>
       </c>
-      <c r="B131" s="52" t="s">
-        <v>5</v>
-      </c>
-      <c r="C131" s="33">
+      <c r="B132" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C132" s="33">
         <v>42156</v>
       </c>
-      <c r="D131" s="52" t="s">
+      <c r="D132" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="E131" s="51">
+      <c r="E132" s="51">
         <v>0.43958333333333338</v>
       </c>
-      <c r="F131" s="51">
+      <c r="F132" s="51">
         <v>0.625</v>
       </c>
-      <c r="G131" s="32"/>
-      <c r="H131" s="35" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8">
-      <c r="A132" s="36" t="str">
+      <c r="G132" s="32"/>
+      <c r="H132" s="35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8">
+      <c r="A133" s="36" t="str">
         <f t="shared" si="3"/>
         <v>Oceano_2015-06-01_BSNE_A4_1033_1500</v>
       </c>
-      <c r="B132" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="C132" s="38">
+      <c r="B133" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C133" s="38">
         <v>42156</v>
       </c>
-      <c r="D132" s="42" t="s">
+      <c r="D133" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="E132" s="41">
+      <c r="E133" s="41">
         <v>0.43958333333333338</v>
       </c>
-      <c r="F132" s="41">
+      <c r="F133" s="41">
         <v>0.625</v>
       </c>
-      <c r="G132" s="37"/>
-      <c r="H132" s="40" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8">
-      <c r="A133" s="44" t="str">
+      <c r="G133" s="37"/>
+      <c r="H133" s="40" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8">
+      <c r="A134" s="44" t="str">
         <f t="shared" si="3"/>
         <v>Oceano_2015-06-01_BSNE_B4_1033_1500</v>
       </c>
-      <c r="B133" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="C133" s="46">
+      <c r="B134" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C134" s="46">
         <v>42156</v>
       </c>
-      <c r="D133" s="45" t="s">
+      <c r="D134" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="E133" s="47">
+      <c r="E134" s="47">
         <v>0.43958333333333338</v>
       </c>
-      <c r="F133" s="47">
+      <c r="F134" s="47">
         <v>0.625</v>
       </c>
-      <c r="G133" s="48"/>
-      <c r="H133" s="49" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8">
-      <c r="A134" s="31" t="str">
+      <c r="G134" s="48"/>
+      <c r="H134" s="49" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8">
+      <c r="A135" s="31" t="str">
         <f t="shared" si="3"/>
         <v>Oceano_2015-06-02_BSNE_A1_1154_1528</v>
       </c>
-      <c r="B134" s="52" t="s">
-        <v>5</v>
-      </c>
-      <c r="C134" s="33">
+      <c r="B135" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C135" s="33">
         <v>42157</v>
       </c>
-      <c r="D134" s="32" t="s">
+      <c r="D135" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="E134" s="51">
+      <c r="E135" s="51">
         <v>0.49583333333333335</v>
       </c>
-      <c r="F134" s="51">
+      <c r="F135" s="51">
         <v>0.64444444444444449</v>
       </c>
-      <c r="G134" s="32" t="s">
+      <c r="G135" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="H134" s="35" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8">
-      <c r="A135" s="36" t="str">
-        <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_A1_1537_1757</v>
-      </c>
-      <c r="B135" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="C135" s="38">
-        <v>42157</v>
-      </c>
-      <c r="D135" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="E135" s="41">
-        <v>0.65069444444444446</v>
-      </c>
-      <c r="F135" s="41">
-        <v>0.74791666666666667</v>
-      </c>
-      <c r="G135" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="H135" s="40" t="s">
+      <c r="H135" s="35" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="136" spans="1:8">
       <c r="A136" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_A2_1154_1528</v>
+        <v>Oceano_2015-06-02_BSNE_A1_1537_1757</v>
       </c>
       <c r="B136" s="42" t="s">
         <v>5</v>
@@ -8451,14 +8457,14 @@
       <c r="C136" s="38">
         <v>42157</v>
       </c>
-      <c r="D136" s="42" t="s">
-        <v>8</v>
+      <c r="D136" s="37" t="s">
+        <v>7</v>
       </c>
       <c r="E136" s="41">
-        <v>0.49583333333333335</v>
+        <v>0.65069444444444446</v>
       </c>
       <c r="F136" s="41">
-        <v>0.64444444444444449</v>
+        <v>0.74791666666666667</v>
       </c>
       <c r="G136" s="37" t="s">
         <v>31</v>
@@ -8470,7 +8476,7 @@
     <row r="137" spans="1:8">
       <c r="A137" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_A2_1537_1757</v>
+        <v>Oceano_2015-06-02_BSNE_A2_1154_1528</v>
       </c>
       <c r="B137" s="42" t="s">
         <v>5</v>
@@ -8482,12 +8488,12 @@
         <v>8</v>
       </c>
       <c r="E137" s="41">
-        <v>0.65069444444444446</v>
+        <v>0.49583333333333335</v>
       </c>
       <c r="F137" s="41">
-        <v>0.74791666666666667</v>
-      </c>
-      <c r="G137" s="42" t="s">
+        <v>0.64444444444444449</v>
+      </c>
+      <c r="G137" s="37" t="s">
         <v>31</v>
       </c>
       <c r="H137" s="40" t="s">
@@ -8497,7 +8503,7 @@
     <row r="138" spans="1:8">
       <c r="A138" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_A3_1154_1254</v>
+        <v>Oceano_2015-06-02_BSNE_A2_1537_1757</v>
       </c>
       <c r="B138" s="42" t="s">
         <v>5</v>
@@ -8506,16 +8512,16 @@
         <v>42157</v>
       </c>
       <c r="D138" s="42" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E138" s="41">
-        <v>0.49583333333333335</v>
+        <v>0.65069444444444446</v>
       </c>
       <c r="F138" s="41">
-        <v>0.53749999999999998</v>
-      </c>
-      <c r="G138" s="37" t="s">
-        <v>27</v>
+        <v>0.74791666666666667</v>
+      </c>
+      <c r="G138" s="42" t="s">
+        <v>31</v>
       </c>
       <c r="H138" s="40" t="s">
         <v>30</v>
@@ -8524,7 +8530,7 @@
     <row r="139" spans="1:8">
       <c r="A139" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_A3_1317_1417</v>
+        <v>Oceano_2015-06-02_BSNE_A3_1154_1254</v>
       </c>
       <c r="B139" s="42" t="s">
         <v>5</v>
@@ -8536,10 +8542,10 @@
         <v>14</v>
       </c>
       <c r="E139" s="41">
-        <v>0.55347222222222225</v>
+        <v>0.49583333333333335</v>
       </c>
       <c r="F139" s="41">
-        <v>0.59513888888888888</v>
+        <v>0.53749999999999998</v>
       </c>
       <c r="G139" s="37" t="s">
         <v>27</v>
@@ -8551,7 +8557,7 @@
     <row r="140" spans="1:8">
       <c r="A140" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_A3_1428_1528</v>
+        <v>Oceano_2015-06-02_BSNE_A3_1317_1417</v>
       </c>
       <c r="B140" s="42" t="s">
         <v>5</v>
@@ -8563,10 +8569,10 @@
         <v>14</v>
       </c>
       <c r="E140" s="41">
-        <v>0.60277777777777775</v>
+        <v>0.55347222222222225</v>
       </c>
       <c r="F140" s="41">
-        <v>0.64444444444444449</v>
+        <v>0.59513888888888888</v>
       </c>
       <c r="G140" s="37" t="s">
         <v>27</v>
@@ -8578,7 +8584,7 @@
     <row r="141" spans="1:8">
       <c r="A141" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_A3_1537_1607</v>
+        <v>Oceano_2015-06-02_BSNE_A3_1428_1528</v>
       </c>
       <c r="B141" s="42" t="s">
         <v>5</v>
@@ -8590,10 +8596,10 @@
         <v>14</v>
       </c>
       <c r="E141" s="41">
-        <v>0.65069444444444446</v>
+        <v>0.60277777777777775</v>
       </c>
       <c r="F141" s="41">
-        <v>0.67152777777777783</v>
+        <v>0.64444444444444449</v>
       </c>
       <c r="G141" s="37" t="s">
         <v>27</v>
@@ -8605,7 +8611,7 @@
     <row r="142" spans="1:8">
       <c r="A142" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_A3_1613_1643</v>
+        <v>Oceano_2015-06-02_BSNE_A3_1537_1607</v>
       </c>
       <c r="B142" s="42" t="s">
         <v>5</v>
@@ -8617,10 +8623,10 @@
         <v>14</v>
       </c>
       <c r="E142" s="41">
-        <v>0.67569444444444438</v>
+        <v>0.65069444444444446</v>
       </c>
       <c r="F142" s="41">
-        <v>0.69652777777777775</v>
+        <v>0.67152777777777783</v>
       </c>
       <c r="G142" s="37" t="s">
         <v>27</v>
@@ -8632,7 +8638,7 @@
     <row r="143" spans="1:8">
       <c r="A143" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_A3_1649_1719</v>
+        <v>Oceano_2015-06-02_BSNE_A3_1613_1643</v>
       </c>
       <c r="B143" s="42" t="s">
         <v>5</v>
@@ -8644,10 +8650,10 @@
         <v>14</v>
       </c>
       <c r="E143" s="41">
-        <v>0.7006944444444444</v>
+        <v>0.67569444444444438</v>
       </c>
       <c r="F143" s="41">
-        <v>0.72152777777777777</v>
+        <v>0.69652777777777775</v>
       </c>
       <c r="G143" s="37" t="s">
         <v>27</v>
@@ -8659,7 +8665,7 @@
     <row r="144" spans="1:8">
       <c r="A144" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_A3_1727_1757</v>
+        <v>Oceano_2015-06-02_BSNE_A3_1649_1719</v>
       </c>
       <c r="B144" s="42" t="s">
         <v>5</v>
@@ -8671,10 +8677,10 @@
         <v>14</v>
       </c>
       <c r="E144" s="41">
-        <v>0.7270833333333333</v>
+        <v>0.7006944444444444</v>
       </c>
       <c r="F144" s="41">
-        <v>0.74791666666666667</v>
+        <v>0.72152777777777777</v>
       </c>
       <c r="G144" s="37" t="s">
         <v>27</v>
@@ -8686,7 +8692,7 @@
     <row r="145" spans="1:8">
       <c r="A145" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_A4_1154_1254</v>
+        <v>Oceano_2015-06-02_BSNE_A3_1727_1757</v>
       </c>
       <c r="B145" s="42" t="s">
         <v>5</v>
@@ -8695,15 +8701,17 @@
         <v>42157</v>
       </c>
       <c r="D145" s="42" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E145" s="41">
-        <v>0.49583333333333335</v>
+        <v>0.7270833333333333</v>
       </c>
       <c r="F145" s="41">
-        <v>0.53749999999999998</v>
-      </c>
-      <c r="G145" s="37"/>
+        <v>0.74791666666666667</v>
+      </c>
+      <c r="G145" s="37" t="s">
+        <v>27</v>
+      </c>
       <c r="H145" s="40" t="s">
         <v>30</v>
       </c>
@@ -8711,7 +8719,7 @@
     <row r="146" spans="1:8">
       <c r="A146" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_A4_1317_1417</v>
+        <v>Oceano_2015-06-02_BSNE_A4_1154_1254</v>
       </c>
       <c r="B146" s="42" t="s">
         <v>5</v>
@@ -8723,10 +8731,10 @@
         <v>15</v>
       </c>
       <c r="E146" s="41">
-        <v>0.55347222222222225</v>
+        <v>0.49583333333333335</v>
       </c>
       <c r="F146" s="41">
-        <v>0.59513888888888888</v>
+        <v>0.53749999999999998</v>
       </c>
       <c r="G146" s="37"/>
       <c r="H146" s="40" t="s">
@@ -8736,7 +8744,7 @@
     <row r="147" spans="1:8">
       <c r="A147" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_A4_1428_1528</v>
+        <v>Oceano_2015-06-02_BSNE_A4_1317_1417</v>
       </c>
       <c r="B147" s="42" t="s">
         <v>5</v>
@@ -8748,14 +8756,12 @@
         <v>15</v>
       </c>
       <c r="E147" s="41">
-        <v>0.60277777777777775</v>
+        <v>0.55347222222222225</v>
       </c>
       <c r="F147" s="41">
-        <v>0.64444444444444449</v>
-      </c>
-      <c r="G147" s="37" t="s">
-        <v>27</v>
-      </c>
+        <v>0.59513888888888888</v>
+      </c>
+      <c r="G147" s="37"/>
       <c r="H147" s="40" t="s">
         <v>30</v>
       </c>
@@ -8763,7 +8769,7 @@
     <row r="148" spans="1:8">
       <c r="A148" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_A4_1537_1607</v>
+        <v>Oceano_2015-06-02_BSNE_A4_1428_1528</v>
       </c>
       <c r="B148" s="42" t="s">
         <v>5</v>
@@ -8775,10 +8781,10 @@
         <v>15</v>
       </c>
       <c r="E148" s="41">
-        <v>0.65069444444444446</v>
+        <v>0.60277777777777775</v>
       </c>
       <c r="F148" s="41">
-        <v>0.67152777777777783</v>
+        <v>0.64444444444444449</v>
       </c>
       <c r="G148" s="37" t="s">
         <v>27</v>
@@ -8790,7 +8796,7 @@
     <row r="149" spans="1:8">
       <c r="A149" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_A4_1613_1643</v>
+        <v>Oceano_2015-06-02_BSNE_A4_1537_1607</v>
       </c>
       <c r="B149" s="42" t="s">
         <v>5</v>
@@ -8802,10 +8808,10 @@
         <v>15</v>
       </c>
       <c r="E149" s="41">
-        <v>0.67569444444444438</v>
+        <v>0.65069444444444446</v>
       </c>
       <c r="F149" s="41">
-        <v>0.69652777777777775</v>
+        <v>0.67152777777777783</v>
       </c>
       <c r="G149" s="37" t="s">
         <v>27</v>
@@ -8817,7 +8823,7 @@
     <row r="150" spans="1:8">
       <c r="A150" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_A4_1649_1719</v>
+        <v>Oceano_2015-06-02_BSNE_A4_1613_1643</v>
       </c>
       <c r="B150" s="42" t="s">
         <v>5</v>
@@ -8829,12 +8835,14 @@
         <v>15</v>
       </c>
       <c r="E150" s="41">
-        <v>0.7006944444444444</v>
+        <v>0.67569444444444438</v>
       </c>
       <c r="F150" s="41">
-        <v>0.72152777777777777</v>
-      </c>
-      <c r="G150" s="37"/>
+        <v>0.69652777777777775</v>
+      </c>
+      <c r="G150" s="37" t="s">
+        <v>27</v>
+      </c>
       <c r="H150" s="40" t="s">
         <v>30</v>
       </c>
@@ -8842,7 +8850,7 @@
     <row r="151" spans="1:8">
       <c r="A151" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_A4_1727_1757</v>
+        <v>Oceano_2015-06-02_BSNE_A4_1649_1719</v>
       </c>
       <c r="B151" s="42" t="s">
         <v>5</v>
@@ -8854,10 +8862,10 @@
         <v>15</v>
       </c>
       <c r="E151" s="41">
-        <v>0.7270833333333333</v>
+        <v>0.7006944444444444</v>
       </c>
       <c r="F151" s="41">
-        <v>0.74791666666666667</v>
+        <v>0.72152777777777777</v>
       </c>
       <c r="G151" s="37"/>
       <c r="H151" s="40" t="s">
@@ -8867,7 +8875,7 @@
     <row r="152" spans="1:8">
       <c r="A152" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_B1_1154_1254</v>
+        <v>Oceano_2015-06-02_BSNE_A4_1727_1757</v>
       </c>
       <c r="B152" s="42" t="s">
         <v>5</v>
@@ -8876,13 +8884,13 @@
         <v>42157</v>
       </c>
       <c r="D152" s="42" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E152" s="41">
-        <v>0.49583333333333335</v>
+        <v>0.7270833333333333</v>
       </c>
       <c r="F152" s="41">
-        <v>0.53749999999999998</v>
+        <v>0.74791666666666667</v>
       </c>
       <c r="G152" s="37"/>
       <c r="H152" s="40" t="s">
@@ -8892,7 +8900,7 @@
     <row r="153" spans="1:8">
       <c r="A153" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_B1_1317_1417</v>
+        <v>Oceano_2015-06-02_BSNE_B1_1154_1254</v>
       </c>
       <c r="B153" s="42" t="s">
         <v>5</v>
@@ -8904,10 +8912,10 @@
         <v>9</v>
       </c>
       <c r="E153" s="41">
-        <v>0.55347222222222225</v>
+        <v>0.49583333333333335</v>
       </c>
       <c r="F153" s="41">
-        <v>0.59513888888888888</v>
+        <v>0.53749999999999998</v>
       </c>
       <c r="G153" s="37"/>
       <c r="H153" s="40" t="s">
@@ -8917,7 +8925,7 @@
     <row r="154" spans="1:8">
       <c r="A154" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_B1_1428_1528</v>
+        <v>Oceano_2015-06-02_BSNE_B1_1317_1417</v>
       </c>
       <c r="B154" s="42" t="s">
         <v>5</v>
@@ -8929,14 +8937,12 @@
         <v>9</v>
       </c>
       <c r="E154" s="41">
-        <v>0.60277777777777775</v>
+        <v>0.55347222222222225</v>
       </c>
       <c r="F154" s="41">
-        <v>0.64444444444444449</v>
-      </c>
-      <c r="G154" s="37" t="s">
-        <v>27</v>
-      </c>
+        <v>0.59513888888888888</v>
+      </c>
+      <c r="G154" s="37"/>
       <c r="H154" s="40" t="s">
         <v>30</v>
       </c>
@@ -8944,7 +8950,7 @@
     <row r="155" spans="1:8">
       <c r="A155" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_B1_1537_1607</v>
+        <v>Oceano_2015-06-02_BSNE_B1_1428_1528</v>
       </c>
       <c r="B155" s="42" t="s">
         <v>5</v>
@@ -8956,10 +8962,10 @@
         <v>9</v>
       </c>
       <c r="E155" s="41">
-        <v>0.65069444444444446</v>
+        <v>0.60277777777777775</v>
       </c>
       <c r="F155" s="41">
-        <v>0.67152777777777783</v>
+        <v>0.64444444444444449</v>
       </c>
       <c r="G155" s="37" t="s">
         <v>27</v>
@@ -8971,7 +8977,7 @@
     <row r="156" spans="1:8">
       <c r="A156" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_B1_1613_1643</v>
+        <v>Oceano_2015-06-02_BSNE_B1_1537_1607</v>
       </c>
       <c r="B156" s="42" t="s">
         <v>5</v>
@@ -8983,12 +8989,14 @@
         <v>9</v>
       </c>
       <c r="E156" s="41">
-        <v>0.67569444444444438</v>
+        <v>0.65069444444444446</v>
       </c>
       <c r="F156" s="41">
-        <v>0.69652777777777775</v>
-      </c>
-      <c r="G156" s="37"/>
+        <v>0.67152777777777783</v>
+      </c>
+      <c r="G156" s="37" t="s">
+        <v>27</v>
+      </c>
       <c r="H156" s="40" t="s">
         <v>30</v>
       </c>
@@ -8996,7 +9004,7 @@
     <row r="157" spans="1:8">
       <c r="A157" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_B1_1649_1719</v>
+        <v>Oceano_2015-06-02_BSNE_B1_1613_1643</v>
       </c>
       <c r="B157" s="42" t="s">
         <v>5</v>
@@ -9008,10 +9016,10 @@
         <v>9</v>
       </c>
       <c r="E157" s="41">
-        <v>0.7006944444444444</v>
+        <v>0.67569444444444438</v>
       </c>
       <c r="F157" s="41">
-        <v>0.72152777777777777</v>
+        <v>0.69652777777777775</v>
       </c>
       <c r="G157" s="37"/>
       <c r="H157" s="40" t="s">
@@ -9021,7 +9029,7 @@
     <row r="158" spans="1:8">
       <c r="A158" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_B1_1727_1757</v>
+        <v>Oceano_2015-06-02_BSNE_B1_1649_1719</v>
       </c>
       <c r="B158" s="42" t="s">
         <v>5</v>
@@ -9033,10 +9041,10 @@
         <v>9</v>
       </c>
       <c r="E158" s="41">
-        <v>0.7270833333333333</v>
+        <v>0.7006944444444444</v>
       </c>
       <c r="F158" s="41">
-        <v>0.74791666666666667</v>
+        <v>0.72152777777777777</v>
       </c>
       <c r="G158" s="37"/>
       <c r="H158" s="40" t="s">
@@ -9046,7 +9054,7 @@
     <row r="159" spans="1:8">
       <c r="A159" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_B2_1154_1254</v>
+        <v>Oceano_2015-06-02_BSNE_B1_1727_1757</v>
       </c>
       <c r="B159" s="42" t="s">
         <v>5</v>
@@ -9055,13 +9063,13 @@
         <v>42157</v>
       </c>
       <c r="D159" s="42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E159" s="41">
-        <v>0.49583333333333335</v>
+        <v>0.7270833333333333</v>
       </c>
       <c r="F159" s="41">
-        <v>0.53749999999999998</v>
+        <v>0.74791666666666667</v>
       </c>
       <c r="G159" s="37"/>
       <c r="H159" s="40" t="s">
@@ -9071,7 +9079,7 @@
     <row r="160" spans="1:8">
       <c r="A160" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_B2_1317_1417</v>
+        <v>Oceano_2015-06-02_BSNE_B2_1154_1254</v>
       </c>
       <c r="B160" s="42" t="s">
         <v>5</v>
@@ -9083,10 +9091,10 @@
         <v>10</v>
       </c>
       <c r="E160" s="41">
-        <v>0.55347222222222225</v>
+        <v>0.49583333333333335</v>
       </c>
       <c r="F160" s="41">
-        <v>0.59513888888888888</v>
+        <v>0.53749999999999998</v>
       </c>
       <c r="G160" s="37"/>
       <c r="H160" s="40" t="s">
@@ -9096,7 +9104,7 @@
     <row r="161" spans="1:8">
       <c r="A161" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_B2_1428_1528</v>
+        <v>Oceano_2015-06-02_BSNE_B2_1317_1417</v>
       </c>
       <c r="B161" s="42" t="s">
         <v>5</v>
@@ -9108,14 +9116,12 @@
         <v>10</v>
       </c>
       <c r="E161" s="41">
-        <v>0.60277777777777775</v>
+        <v>0.55347222222222225</v>
       </c>
       <c r="F161" s="41">
-        <v>0.64444444444444449</v>
-      </c>
-      <c r="G161" s="37" t="s">
-        <v>27</v>
-      </c>
+        <v>0.59513888888888888</v>
+      </c>
+      <c r="G161" s="37"/>
       <c r="H161" s="40" t="s">
         <v>30</v>
       </c>
@@ -9123,7 +9129,7 @@
     <row r="162" spans="1:8">
       <c r="A162" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_B2_1537_1607</v>
+        <v>Oceano_2015-06-02_BSNE_B2_1428_1528</v>
       </c>
       <c r="B162" s="42" t="s">
         <v>5</v>
@@ -9135,10 +9141,10 @@
         <v>10</v>
       </c>
       <c r="E162" s="41">
-        <v>0.65069444444444446</v>
+        <v>0.60277777777777775</v>
       </c>
       <c r="F162" s="41">
-        <v>0.67152777777777783</v>
+        <v>0.64444444444444449</v>
       </c>
       <c r="G162" s="37" t="s">
         <v>27</v>
@@ -9150,7 +9156,7 @@
     <row r="163" spans="1:8">
       <c r="A163" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_B2_1613_1643</v>
+        <v>Oceano_2015-06-02_BSNE_B2_1537_1607</v>
       </c>
       <c r="B163" s="42" t="s">
         <v>5</v>
@@ -9162,10 +9168,10 @@
         <v>10</v>
       </c>
       <c r="E163" s="41">
-        <v>0.67569444444444438</v>
+        <v>0.65069444444444446</v>
       </c>
       <c r="F163" s="41">
-        <v>0.69652777777777775</v>
+        <v>0.67152777777777783</v>
       </c>
       <c r="G163" s="37" t="s">
         <v>27</v>
@@ -9177,7 +9183,7 @@
     <row r="164" spans="1:8">
       <c r="A164" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_B2_1649_1719</v>
+        <v>Oceano_2015-06-02_BSNE_B2_1613_1643</v>
       </c>
       <c r="B164" s="42" t="s">
         <v>5</v>
@@ -9189,12 +9195,14 @@
         <v>10</v>
       </c>
       <c r="E164" s="41">
-        <v>0.7006944444444444</v>
+        <v>0.67569444444444438</v>
       </c>
       <c r="F164" s="41">
-        <v>0.72152777777777777</v>
-      </c>
-      <c r="G164" s="37"/>
+        <v>0.69652777777777775</v>
+      </c>
+      <c r="G164" s="37" t="s">
+        <v>27</v>
+      </c>
       <c r="H164" s="40" t="s">
         <v>30</v>
       </c>
@@ -9202,7 +9210,7 @@
     <row r="165" spans="1:8">
       <c r="A165" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_B2_1727_1757</v>
+        <v>Oceano_2015-06-02_BSNE_B2_1649_1719</v>
       </c>
       <c r="B165" s="42" t="s">
         <v>5</v>
@@ -9214,10 +9222,10 @@
         <v>10</v>
       </c>
       <c r="E165" s="41">
-        <v>0.7270833333333333</v>
+        <v>0.7006944444444444</v>
       </c>
       <c r="F165" s="41">
-        <v>0.74791666666666667</v>
+        <v>0.72152777777777777</v>
       </c>
       <c r="G165" s="37"/>
       <c r="H165" s="40" t="s">
@@ -9227,7 +9235,7 @@
     <row r="166" spans="1:8">
       <c r="A166" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_B3_1154_1757</v>
+        <v>Oceano_2015-06-02_BSNE_B2_1727_1757</v>
       </c>
       <c r="B166" s="42" t="s">
         <v>5</v>
@@ -9236,17 +9244,15 @@
         <v>42157</v>
       </c>
       <c r="D166" s="42" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E166" s="41">
-        <v>0.49583333333333335</v>
+        <v>0.7270833333333333</v>
       </c>
       <c r="F166" s="41">
         <v>0.74791666666666667</v>
       </c>
-      <c r="G166" s="42" t="s">
-        <v>31</v>
-      </c>
+      <c r="G166" s="37"/>
       <c r="H166" s="40" t="s">
         <v>30</v>
       </c>
@@ -9254,7 +9260,7 @@
     <row r="167" spans="1:8">
       <c r="A167" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_B4_1154_1254</v>
+        <v>Oceano_2015-06-02_BSNE_B3_1154_1757</v>
       </c>
       <c r="B167" s="42" t="s">
         <v>5</v>
@@ -9263,15 +9269,17 @@
         <v>42157</v>
       </c>
       <c r="D167" s="42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E167" s="41">
         <v>0.49583333333333335</v>
       </c>
       <c r="F167" s="41">
-        <v>0.53749999999999998</v>
-      </c>
-      <c r="G167" s="37"/>
+        <v>0.74791666666666667</v>
+      </c>
+      <c r="G167" s="42" t="s">
+        <v>31</v>
+      </c>
       <c r="H167" s="40" t="s">
         <v>30</v>
       </c>
@@ -9279,7 +9287,7 @@
     <row r="168" spans="1:8">
       <c r="A168" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_B4_1317_1417</v>
+        <v>Oceano_2015-06-02_BSNE_B4_1154_1254</v>
       </c>
       <c r="B168" s="42" t="s">
         <v>5</v>
@@ -9291,10 +9299,10 @@
         <v>17</v>
       </c>
       <c r="E168" s="41">
-        <v>0.55347222222222225</v>
+        <v>0.49583333333333335</v>
       </c>
       <c r="F168" s="41">
-        <v>0.59513888888888888</v>
+        <v>0.53749999999999998</v>
       </c>
       <c r="G168" s="37"/>
       <c r="H168" s="40" t="s">
@@ -9304,7 +9312,7 @@
     <row r="169" spans="1:8">
       <c r="A169" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_B4_1428_1528</v>
+        <v>Oceano_2015-06-02_BSNE_B4_1317_1417</v>
       </c>
       <c r="B169" s="42" t="s">
         <v>5</v>
@@ -9316,14 +9324,12 @@
         <v>17</v>
       </c>
       <c r="E169" s="41">
-        <v>0.60277777777777775</v>
+        <v>0.55347222222222225</v>
       </c>
       <c r="F169" s="41">
-        <v>0.64444444444444449</v>
-      </c>
-      <c r="G169" s="37" t="s">
-        <v>27</v>
-      </c>
+        <v>0.59513888888888888</v>
+      </c>
+      <c r="G169" s="37"/>
       <c r="H169" s="40" t="s">
         <v>30</v>
       </c>
@@ -9331,7 +9337,7 @@
     <row r="170" spans="1:8">
       <c r="A170" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_B4_1537_1607</v>
+        <v>Oceano_2015-06-02_BSNE_B4_1428_1528</v>
       </c>
       <c r="B170" s="42" t="s">
         <v>5</v>
@@ -9343,10 +9349,10 @@
         <v>17</v>
       </c>
       <c r="E170" s="41">
-        <v>0.65069444444444446</v>
+        <v>0.60277777777777775</v>
       </c>
       <c r="F170" s="41">
-        <v>0.67152777777777783</v>
+        <v>0.64444444444444449</v>
       </c>
       <c r="G170" s="37" t="s">
         <v>27</v>
@@ -9358,7 +9364,7 @@
     <row r="171" spans="1:8">
       <c r="A171" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_B4_1613_1643</v>
+        <v>Oceano_2015-06-02_BSNE_B4_1537_1607</v>
       </c>
       <c r="B171" s="42" t="s">
         <v>5</v>
@@ -9370,10 +9376,10 @@
         <v>17</v>
       </c>
       <c r="E171" s="41">
-        <v>0.67569444444444438</v>
+        <v>0.65069444444444446</v>
       </c>
       <c r="F171" s="41">
-        <v>0.69652777777777775</v>
+        <v>0.67152777777777783</v>
       </c>
       <c r="G171" s="37" t="s">
         <v>27</v>
@@ -9385,7 +9391,7 @@
     <row r="172" spans="1:8">
       <c r="A172" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-02_BSNE_B4_1649_1719</v>
+        <v>Oceano_2015-06-02_BSNE_B4_1613_1643</v>
       </c>
       <c r="B172" s="42" t="s">
         <v>5</v>
@@ -9397,10 +9403,10 @@
         <v>17</v>
       </c>
       <c r="E172" s="41">
-        <v>0.7006944444444444</v>
+        <v>0.67569444444444438</v>
       </c>
       <c r="F172" s="41">
-        <v>0.72152777777777777</v>
+        <v>0.69652777777777775</v>
       </c>
       <c r="G172" s="37" t="s">
         <v>27</v>
@@ -9410,90 +9416,90 @@
       </c>
     </row>
     <row r="173" spans="1:8">
-      <c r="A173" s="44" t="str">
+      <c r="A173" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v>Oceano_2015-06-02_BSNE_B4_1649_1719</v>
+      </c>
+      <c r="B173" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C173" s="38">
+        <v>42157</v>
+      </c>
+      <c r="D173" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="E173" s="41">
+        <v>0.7006944444444444</v>
+      </c>
+      <c r="F173" s="41">
+        <v>0.72152777777777777</v>
+      </c>
+      <c r="G173" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="H173" s="40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8">
+      <c r="A174" s="44" t="str">
         <f t="shared" si="3"/>
         <v>Oceano_2015-06-02_BSNE_B4_1727_1757</v>
       </c>
-      <c r="B173" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="C173" s="46">
+      <c r="B174" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C174" s="46">
         <v>42157</v>
       </c>
-      <c r="D173" s="45" t="s">
+      <c r="D174" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="E173" s="47">
+      <c r="E174" s="47">
         <v>0.7270833333333333</v>
       </c>
-      <c r="F173" s="47">
+      <c r="F174" s="47">
         <v>0.74791666666666667</v>
       </c>
-      <c r="G173" s="48" t="s">
+      <c r="G174" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="H173" s="49" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="174" spans="1:8">
-      <c r="A174" s="31" t="str">
+      <c r="H174" s="49" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8">
+      <c r="A175" s="31" t="str">
         <f t="shared" si="3"/>
         <v>Oceano_2015-06-03_BSNE_A1_1040_1514</v>
       </c>
-      <c r="B174" s="52" t="s">
-        <v>5</v>
-      </c>
-      <c r="C174" s="33">
+      <c r="B175" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C175" s="33">
         <v>42158</v>
       </c>
-      <c r="D174" s="32" t="s">
+      <c r="D175" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="E174" s="51">
+      <c r="E175" s="51">
         <v>0.44444444444444442</v>
       </c>
-      <c r="F174" s="51">
+      <c r="F175" s="51">
         <v>0.63472222222222219</v>
       </c>
-      <c r="G174" s="32" t="s">
+      <c r="G175" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="H174" s="35" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="175" spans="1:8">
-      <c r="A175" s="36" t="str">
-        <f t="shared" si="3"/>
-        <v>Oceano_2015-06-03_BSNE_A1_1520_1813</v>
-      </c>
-      <c r="B175" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="C175" s="38">
-        <v>42158</v>
-      </c>
-      <c r="D175" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="E175" s="41">
-        <v>0.63888888888888895</v>
-      </c>
-      <c r="F175" s="41">
-        <v>0.75902777777777775</v>
-      </c>
-      <c r="G175" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="H175" s="40" t="s">
+      <c r="H175" s="35" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="176" spans="1:8">
       <c r="A176" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-03_BSNE_A2_1040_1514</v>
+        <v>Oceano_2015-06-03_BSNE_A1_1520_1813</v>
       </c>
       <c r="B176" s="42" t="s">
         <v>5</v>
@@ -9501,14 +9507,14 @@
       <c r="C176" s="38">
         <v>42158</v>
       </c>
-      <c r="D176" s="42" t="s">
-        <v>8</v>
+      <c r="D176" s="37" t="s">
+        <v>7</v>
       </c>
       <c r="E176" s="41">
-        <v>0.44444444444444442</v>
+        <v>0.63888888888888895</v>
       </c>
       <c r="F176" s="41">
-        <v>0.63472222222222219</v>
+        <v>0.75902777777777775</v>
       </c>
       <c r="G176" s="42" t="s">
         <v>31</v>
@@ -9520,7 +9526,7 @@
     <row r="177" spans="1:8">
       <c r="A177" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-03_BSNE_A2_1520_1813</v>
+        <v>Oceano_2015-06-03_BSNE_A2_1040_1514</v>
       </c>
       <c r="B177" s="42" t="s">
         <v>5</v>
@@ -9532,10 +9538,10 @@
         <v>8</v>
       </c>
       <c r="E177" s="41">
-        <v>0.63888888888888895</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="F177" s="41">
-        <v>0.75902777777777775</v>
+        <v>0.63472222222222219</v>
       </c>
       <c r="G177" s="42" t="s">
         <v>31</v>
@@ -9547,7 +9553,7 @@
     <row r="178" spans="1:8">
       <c r="A178" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-03_BSNE_A3_1040_1345</v>
+        <v>Oceano_2015-06-03_BSNE_A2_1520_1813</v>
       </c>
       <c r="B178" s="42" t="s">
         <v>5</v>
@@ -9556,15 +9562,17 @@
         <v>42158</v>
       </c>
       <c r="D178" s="42" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E178" s="41">
-        <v>0.44444444444444442</v>
+        <v>0.63888888888888895</v>
       </c>
       <c r="F178" s="41">
-        <v>0.57291666666666663</v>
-      </c>
-      <c r="G178" s="37"/>
+        <v>0.75902777777777775</v>
+      </c>
+      <c r="G178" s="42" t="s">
+        <v>31</v>
+      </c>
       <c r="H178" s="40" t="s">
         <v>29</v>
       </c>
@@ -9572,7 +9580,7 @@
     <row r="179" spans="1:8">
       <c r="A179" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-03_BSNE_A3_1352_1437</v>
+        <v>Oceano_2015-06-03_BSNE_A3_1040_1345</v>
       </c>
       <c r="B179" s="42" t="s">
         <v>5</v>
@@ -9584,14 +9592,12 @@
         <v>14</v>
       </c>
       <c r="E179" s="41">
-        <v>0.57777777777777783</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="F179" s="41">
-        <v>0.60902777777777783</v>
-      </c>
-      <c r="G179" s="37" t="s">
-        <v>27</v>
-      </c>
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="G179" s="37"/>
       <c r="H179" s="40" t="s">
         <v>29</v>
       </c>
@@ -9599,7 +9605,7 @@
     <row r="180" spans="1:8">
       <c r="A180" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-03_BSNE_A3_1444_1514</v>
+        <v>Oceano_2015-06-03_BSNE_A3_1352_1437</v>
       </c>
       <c r="B180" s="42" t="s">
         <v>5</v>
@@ -9611,10 +9617,10 @@
         <v>14</v>
       </c>
       <c r="E180" s="41">
-        <v>0.61388888888888882</v>
+        <v>0.57777777777777783</v>
       </c>
       <c r="F180" s="41">
-        <v>0.63472222222222219</v>
+        <v>0.60902777777777783</v>
       </c>
       <c r="G180" s="37" t="s">
         <v>27</v>
@@ -9626,7 +9632,7 @@
     <row r="181" spans="1:8">
       <c r="A181" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-03_BSNE_A3_1520_1550</v>
+        <v>Oceano_2015-06-03_BSNE_A3_1444_1514</v>
       </c>
       <c r="B181" s="42" t="s">
         <v>5</v>
@@ -9638,10 +9644,10 @@
         <v>14</v>
       </c>
       <c r="E181" s="41">
-        <v>0.63888888888888895</v>
+        <v>0.61388888888888882</v>
       </c>
       <c r="F181" s="41">
-        <v>0.65972222222222221</v>
+        <v>0.63472222222222219</v>
       </c>
       <c r="G181" s="37" t="s">
         <v>27</v>
@@ -9653,7 +9659,7 @@
     <row r="182" spans="1:8">
       <c r="A182" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-03_BSNE_A3_1556_1626</v>
+        <v>Oceano_2015-06-03_BSNE_A3_1520_1550</v>
       </c>
       <c r="B182" s="42" t="s">
         <v>5</v>
@@ -9665,10 +9671,10 @@
         <v>14</v>
       </c>
       <c r="E182" s="41">
-        <v>0.66388888888888886</v>
+        <v>0.63888888888888895</v>
       </c>
       <c r="F182" s="41">
-        <v>0.68472222222222223</v>
+        <v>0.65972222222222221</v>
       </c>
       <c r="G182" s="37" t="s">
         <v>27</v>
@@ -9680,7 +9686,7 @@
     <row r="183" spans="1:8">
       <c r="A183" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-03_BSNE_A3_1632_1702</v>
+        <v>Oceano_2015-06-03_BSNE_A3_1556_1626</v>
       </c>
       <c r="B183" s="42" t="s">
         <v>5</v>
@@ -9692,10 +9698,10 @@
         <v>14</v>
       </c>
       <c r="E183" s="41">
-        <v>0.68888888888888899</v>
+        <v>0.66388888888888886</v>
       </c>
       <c r="F183" s="41">
-        <v>0.70972222222222225</v>
+        <v>0.68472222222222223</v>
       </c>
       <c r="G183" s="37" t="s">
         <v>27</v>
@@ -9707,7 +9713,7 @@
     <row r="184" spans="1:8">
       <c r="A184" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-03_BSNE_A3_1707_1737</v>
+        <v>Oceano_2015-06-03_BSNE_A3_1632_1702</v>
       </c>
       <c r="B184" s="42" t="s">
         <v>5</v>
@@ -9719,10 +9725,10 @@
         <v>14</v>
       </c>
       <c r="E184" s="41">
-        <v>0.71319444444444446</v>
+        <v>0.68888888888888899</v>
       </c>
       <c r="F184" s="41">
-        <v>0.73402777777777783</v>
+        <v>0.70972222222222225</v>
       </c>
       <c r="G184" s="37" t="s">
         <v>27</v>
@@ -9734,7 +9740,7 @@
     <row r="185" spans="1:8">
       <c r="A185" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-03_BSNE_A3_1743_1813</v>
+        <v>Oceano_2015-06-03_BSNE_A3_1707_1737</v>
       </c>
       <c r="B185" s="42" t="s">
         <v>5</v>
@@ -9746,12 +9752,14 @@
         <v>14</v>
       </c>
       <c r="E185" s="41">
-        <v>0.73819444444444438</v>
+        <v>0.71319444444444446</v>
       </c>
       <c r="F185" s="41">
-        <v>0.75902777777777775</v>
-      </c>
-      <c r="G185" s="37"/>
+        <v>0.73402777777777783</v>
+      </c>
+      <c r="G185" s="37" t="s">
+        <v>27</v>
+      </c>
       <c r="H185" s="40" t="s">
         <v>29</v>
       </c>
@@ -9759,7 +9767,7 @@
     <row r="186" spans="1:8">
       <c r="A186" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-03_BSNE_A4_1040_1345</v>
+        <v>Oceano_2015-06-03_BSNE_A3_1743_1813</v>
       </c>
       <c r="B186" s="42" t="s">
         <v>5</v>
@@ -9768,13 +9776,13 @@
         <v>42158</v>
       </c>
       <c r="D186" s="42" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E186" s="41">
-        <v>0.44444444444444442</v>
+        <v>0.73819444444444438</v>
       </c>
       <c r="F186" s="41">
-        <v>0.57291666666666663</v>
+        <v>0.75902777777777775</v>
       </c>
       <c r="G186" s="37"/>
       <c r="H186" s="40" t="s">
@@ -9784,7 +9792,7 @@
     <row r="187" spans="1:8">
       <c r="A187" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-03_BSNE_A4_1352_1437</v>
+        <v>Oceano_2015-06-03_BSNE_A4_1040_1345</v>
       </c>
       <c r="B187" s="42" t="s">
         <v>5</v>
@@ -9796,14 +9804,12 @@
         <v>15</v>
       </c>
       <c r="E187" s="41">
-        <v>0.57777777777777783</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="F187" s="41">
-        <v>0.60902777777777783</v>
-      </c>
-      <c r="G187" s="37" t="s">
-        <v>27</v>
-      </c>
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="G187" s="37"/>
       <c r="H187" s="40" t="s">
         <v>29</v>
       </c>
@@ -9811,7 +9817,7 @@
     <row r="188" spans="1:8">
       <c r="A188" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-03_BSNE_A4_1444_1514</v>
+        <v>Oceano_2015-06-03_BSNE_A4_1352_1437</v>
       </c>
       <c r="B188" s="42" t="s">
         <v>5</v>
@@ -9823,10 +9829,10 @@
         <v>15</v>
       </c>
       <c r="E188" s="41">
-        <v>0.61388888888888882</v>
+        <v>0.57777777777777783</v>
       </c>
       <c r="F188" s="41">
-        <v>0.63472222222222219</v>
+        <v>0.60902777777777783</v>
       </c>
       <c r="G188" s="37" t="s">
         <v>27</v>
@@ -9838,7 +9844,7 @@
     <row r="189" spans="1:8">
       <c r="A189" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-03_BSNE_A4_1520_1550</v>
+        <v>Oceano_2015-06-03_BSNE_A4_1444_1514</v>
       </c>
       <c r="B189" s="42" t="s">
         <v>5</v>
@@ -9850,10 +9856,10 @@
         <v>15</v>
       </c>
       <c r="E189" s="41">
-        <v>0.63888888888888895</v>
+        <v>0.61388888888888882</v>
       </c>
       <c r="F189" s="41">
-        <v>0.65972222222222221</v>
+        <v>0.63472222222222219</v>
       </c>
       <c r="G189" s="37" t="s">
         <v>27</v>
@@ -9865,7 +9871,7 @@
     <row r="190" spans="1:8">
       <c r="A190" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-03_BSNE_A4_1556_1626</v>
+        <v>Oceano_2015-06-03_BSNE_A4_1520_1550</v>
       </c>
       <c r="B190" s="42" t="s">
         <v>5</v>
@@ -9877,12 +9883,14 @@
         <v>15</v>
       </c>
       <c r="E190" s="41">
-        <v>0.66388888888888886</v>
+        <v>0.63888888888888895</v>
       </c>
       <c r="F190" s="41">
-        <v>0.68472222222222223</v>
-      </c>
-      <c r="G190" s="37"/>
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="G190" s="37" t="s">
+        <v>27</v>
+      </c>
       <c r="H190" s="40" t="s">
         <v>29</v>
       </c>
@@ -9890,7 +9898,7 @@
     <row r="191" spans="1:8">
       <c r="A191" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-03_BSNE_A4_1632_1702</v>
+        <v>Oceano_2015-06-03_BSNE_A4_1556_1626</v>
       </c>
       <c r="B191" s="42" t="s">
         <v>5</v>
@@ -9902,10 +9910,10 @@
         <v>15</v>
       </c>
       <c r="E191" s="41">
-        <v>0.68888888888888899</v>
+        <v>0.66388888888888886</v>
       </c>
       <c r="F191" s="41">
-        <v>0.70972222222222225</v>
+        <v>0.68472222222222223</v>
       </c>
       <c r="G191" s="37"/>
       <c r="H191" s="40" t="s">
@@ -9915,7 +9923,7 @@
     <row r="192" spans="1:8">
       <c r="A192" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-03_BSNE_A4_1707_1737</v>
+        <v>Oceano_2015-06-03_BSNE_A4_1632_1702</v>
       </c>
       <c r="B192" s="42" t="s">
         <v>5</v>
@@ -9927,10 +9935,10 @@
         <v>15</v>
       </c>
       <c r="E192" s="41">
-        <v>0.71319444444444446</v>
+        <v>0.68888888888888899</v>
       </c>
       <c r="F192" s="41">
-        <v>0.73402777777777783</v>
+        <v>0.70972222222222225</v>
       </c>
       <c r="G192" s="37"/>
       <c r="H192" s="40" t="s">
@@ -9940,7 +9948,7 @@
     <row r="193" spans="1:8">
       <c r="A193" s="36" t="str">
         <f t="shared" si="3"/>
-        <v>Oceano_2015-06-03_BSNE_A4_1743_1813</v>
+        <v>Oceano_2015-06-03_BSNE_A4_1707_1737</v>
       </c>
       <c r="B193" s="42" t="s">
         <v>5</v>
@@ -9952,10 +9960,10 @@
         <v>15</v>
       </c>
       <c r="E193" s="41">
-        <v>0.73819444444444438</v>
+        <v>0.71319444444444446</v>
       </c>
       <c r="F193" s="41">
-        <v>0.75902777777777775</v>
+        <v>0.73402777777777783</v>
       </c>
       <c r="G193" s="37"/>
       <c r="H193" s="40" t="s">
@@ -9964,8 +9972,8 @@
     </row>
     <row r="194" spans="1:8">
       <c r="A194" s="36" t="str">
-        <f t="shared" ref="A194:A220" si="4">B194&amp;"_"&amp;TEXT(C194,"yyyy-mm-dd")&amp;"_BSNE_"&amp;D194&amp;"_"&amp;TEXT(E194,"HHMM")&amp;"_"&amp;TEXT(F194,"HHMM")</f>
-        <v>Oceano_2015-06-03_BSNE_B1_1040_1345</v>
+        <f t="shared" si="3"/>
+        <v>Oceano_2015-06-03_BSNE_A4_1743_1813</v>
       </c>
       <c r="B194" s="42" t="s">
         <v>5</v>
@@ -9974,13 +9982,13 @@
         <v>42158</v>
       </c>
       <c r="D194" s="42" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E194" s="41">
-        <v>0.44444444444444442</v>
+        <v>0.73819444444444438</v>
       </c>
       <c r="F194" s="41">
-        <v>0.57291666666666663</v>
+        <v>0.75902777777777775</v>
       </c>
       <c r="G194" s="37"/>
       <c r="H194" s="40" t="s">
@@ -9989,8 +9997,8 @@
     </row>
     <row r="195" spans="1:8">
       <c r="A195" s="36" t="str">
-        <f t="shared" si="4"/>
-        <v>Oceano_2015-06-03_BSNE_B1_1352_1437</v>
+        <f t="shared" ref="A195:A221" si="4">B195&amp;"_"&amp;TEXT(C195,"yyyy-mm-dd")&amp;"_BSNE_"&amp;D195&amp;"_"&amp;TEXT(E195,"HHMM")&amp;"_"&amp;TEXT(F195,"HHMM")</f>
+        <v>Oceano_2015-06-03_BSNE_B1_1040_1345</v>
       </c>
       <c r="B195" s="42" t="s">
         <v>5</v>
@@ -10002,10 +10010,10 @@
         <v>9</v>
       </c>
       <c r="E195" s="41">
-        <v>0.57777777777777783</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="F195" s="41">
-        <v>0.60902777777777783</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="G195" s="37"/>
       <c r="H195" s="40" t="s">
@@ -10015,7 +10023,7 @@
     <row r="196" spans="1:8">
       <c r="A196" s="36" t="str">
         <f t="shared" si="4"/>
-        <v>Oceano_2015-06-03_BSNE_B1_1444_1514</v>
+        <v>Oceano_2015-06-03_BSNE_B1_1352_1437</v>
       </c>
       <c r="B196" s="42" t="s">
         <v>5</v>
@@ -10027,10 +10035,10 @@
         <v>9</v>
       </c>
       <c r="E196" s="41">
-        <v>0.61388888888888882</v>
+        <v>0.57777777777777783</v>
       </c>
       <c r="F196" s="41">
-        <v>0.63472222222222219</v>
+        <v>0.60902777777777783</v>
       </c>
       <c r="G196" s="37"/>
       <c r="H196" s="40" t="s">
@@ -10040,7 +10048,7 @@
     <row r="197" spans="1:8">
       <c r="A197" s="36" t="str">
         <f t="shared" si="4"/>
-        <v>Oceano_2015-06-03_BSNE_B1_1520_1550</v>
+        <v>Oceano_2015-06-03_BSNE_B1_1444_1514</v>
       </c>
       <c r="B197" s="42" t="s">
         <v>5</v>
@@ -10052,10 +10060,10 @@
         <v>9</v>
       </c>
       <c r="E197" s="41">
-        <v>0.63888888888888895</v>
+        <v>0.61388888888888882</v>
       </c>
       <c r="F197" s="41">
-        <v>0.65972222222222221</v>
+        <v>0.63472222222222219</v>
       </c>
       <c r="G197" s="37"/>
       <c r="H197" s="40" t="s">
@@ -10065,7 +10073,7 @@
     <row r="198" spans="1:8">
       <c r="A198" s="36" t="str">
         <f t="shared" si="4"/>
-        <v>Oceano_2015-06-03_BSNE_B1_1556_1626</v>
+        <v>Oceano_2015-06-03_BSNE_B1_1520_1550</v>
       </c>
       <c r="B198" s="42" t="s">
         <v>5</v>
@@ -10077,10 +10085,10 @@
         <v>9</v>
       </c>
       <c r="E198" s="41">
-        <v>0.66388888888888886</v>
+        <v>0.63888888888888895</v>
       </c>
       <c r="F198" s="41">
-        <v>0.68472222222222223</v>
+        <v>0.65972222222222221</v>
       </c>
       <c r="G198" s="37"/>
       <c r="H198" s="40" t="s">
@@ -10090,7 +10098,7 @@
     <row r="199" spans="1:8">
       <c r="A199" s="36" t="str">
         <f t="shared" si="4"/>
-        <v>Oceano_2015-06-03_BSNE_B1_1632_1702</v>
+        <v>Oceano_2015-06-03_BSNE_B1_1556_1626</v>
       </c>
       <c r="B199" s="42" t="s">
         <v>5</v>
@@ -10102,10 +10110,10 @@
         <v>9</v>
       </c>
       <c r="E199" s="41">
-        <v>0.68888888888888899</v>
+        <v>0.66388888888888886</v>
       </c>
       <c r="F199" s="41">
-        <v>0.70972222222222225</v>
+        <v>0.68472222222222223</v>
       </c>
       <c r="G199" s="37"/>
       <c r="H199" s="40" t="s">
@@ -10115,7 +10123,7 @@
     <row r="200" spans="1:8">
       <c r="A200" s="36" t="str">
         <f t="shared" si="4"/>
-        <v>Oceano_2015-06-03_BSNE_B1_1707_1737</v>
+        <v>Oceano_2015-06-03_BSNE_B1_1632_1702</v>
       </c>
       <c r="B200" s="42" t="s">
         <v>5</v>
@@ -10127,10 +10135,10 @@
         <v>9</v>
       </c>
       <c r="E200" s="41">
-        <v>0.71319444444444446</v>
+        <v>0.68888888888888899</v>
       </c>
       <c r="F200" s="41">
-        <v>0.73402777777777783</v>
+        <v>0.70972222222222225</v>
       </c>
       <c r="G200" s="37"/>
       <c r="H200" s="40" t="s">
@@ -10140,7 +10148,7 @@
     <row r="201" spans="1:8">
       <c r="A201" s="36" t="str">
         <f t="shared" si="4"/>
-        <v>Oceano_2015-06-03_BSNE_B1_1743_1813</v>
+        <v>Oceano_2015-06-03_BSNE_B1_1707_1737</v>
       </c>
       <c r="B201" s="42" t="s">
         <v>5</v>
@@ -10152,10 +10160,10 @@
         <v>9</v>
       </c>
       <c r="E201" s="41">
-        <v>0.73819444444444438</v>
+        <v>0.71319444444444446</v>
       </c>
       <c r="F201" s="41">
-        <v>0.75902777777777775</v>
+        <v>0.73402777777777783</v>
       </c>
       <c r="G201" s="37"/>
       <c r="H201" s="40" t="s">
@@ -10165,7 +10173,7 @@
     <row r="202" spans="1:8">
       <c r="A202" s="36" t="str">
         <f t="shared" si="4"/>
-        <v>Oceano_2015-06-03_BSNE_B2_1040_1345</v>
+        <v>Oceano_2015-06-03_BSNE_B1_1743_1813</v>
       </c>
       <c r="B202" s="42" t="s">
         <v>5</v>
@@ -10174,13 +10182,13 @@
         <v>42158</v>
       </c>
       <c r="D202" s="42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E202" s="41">
-        <v>0.44444444444444442</v>
+        <v>0.73819444444444438</v>
       </c>
       <c r="F202" s="41">
-        <v>0.57291666666666663</v>
+        <v>0.75902777777777775</v>
       </c>
       <c r="G202" s="37"/>
       <c r="H202" s="40" t="s">
@@ -10190,7 +10198,7 @@
     <row r="203" spans="1:8">
       <c r="A203" s="36" t="str">
         <f t="shared" si="4"/>
-        <v>Oceano_2015-06-03_BSNE_B2_1352_1437</v>
+        <v>Oceano_2015-06-03_BSNE_B2_1040_1345</v>
       </c>
       <c r="B203" s="42" t="s">
         <v>5</v>
@@ -10202,10 +10210,10 @@
         <v>10</v>
       </c>
       <c r="E203" s="41">
-        <v>0.57777777777777783</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="F203" s="41">
-        <v>0.60902777777777783</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="G203" s="37"/>
       <c r="H203" s="40" t="s">
@@ -10215,7 +10223,7 @@
     <row r="204" spans="1:8">
       <c r="A204" s="36" t="str">
         <f t="shared" si="4"/>
-        <v>Oceano_2015-06-03_BSNE_B2_1444_1514</v>
+        <v>Oceano_2015-06-03_BSNE_B2_1352_1437</v>
       </c>
       <c r="B204" s="42" t="s">
         <v>5</v>
@@ -10227,10 +10235,10 @@
         <v>10</v>
       </c>
       <c r="E204" s="41">
-        <v>0.61388888888888882</v>
+        <v>0.57777777777777783</v>
       </c>
       <c r="F204" s="41">
-        <v>0.63472222222222219</v>
+        <v>0.60902777777777783</v>
       </c>
       <c r="G204" s="37"/>
       <c r="H204" s="40" t="s">
@@ -10240,7 +10248,7 @@
     <row r="205" spans="1:8">
       <c r="A205" s="36" t="str">
         <f t="shared" si="4"/>
-        <v>Oceano_2015-06-03_BSNE_B2_1520_1550</v>
+        <v>Oceano_2015-06-03_BSNE_B2_1444_1514</v>
       </c>
       <c r="B205" s="42" t="s">
         <v>5</v>
@@ -10252,10 +10260,10 @@
         <v>10</v>
       </c>
       <c r="E205" s="41">
-        <v>0.63888888888888895</v>
+        <v>0.61388888888888882</v>
       </c>
       <c r="F205" s="41">
-        <v>0.65972222222222221</v>
+        <v>0.63472222222222219</v>
       </c>
       <c r="G205" s="37"/>
       <c r="H205" s="40" t="s">
@@ -10265,7 +10273,7 @@
     <row r="206" spans="1:8">
       <c r="A206" s="36" t="str">
         <f t="shared" si="4"/>
-        <v>Oceano_2015-06-03_BSNE_B2_1556_1626</v>
+        <v>Oceano_2015-06-03_BSNE_B2_1520_1550</v>
       </c>
       <c r="B206" s="42" t="s">
         <v>5</v>
@@ -10277,10 +10285,10 @@
         <v>10</v>
       </c>
       <c r="E206" s="41">
-        <v>0.66388888888888886</v>
+        <v>0.63888888888888895</v>
       </c>
       <c r="F206" s="41">
-        <v>0.68472222222222223</v>
+        <v>0.65972222222222221</v>
       </c>
       <c r="G206" s="37"/>
       <c r="H206" s="40" t="s">
@@ -10290,7 +10298,7 @@
     <row r="207" spans="1:8">
       <c r="A207" s="36" t="str">
         <f t="shared" si="4"/>
-        <v>Oceano_2015-06-03_BSNE_B2_1632_1702</v>
+        <v>Oceano_2015-06-03_BSNE_B2_1556_1626</v>
       </c>
       <c r="B207" s="42" t="s">
         <v>5</v>
@@ -10302,10 +10310,10 @@
         <v>10</v>
       </c>
       <c r="E207" s="41">
-        <v>0.68888888888888899</v>
+        <v>0.66388888888888886</v>
       </c>
       <c r="F207" s="41">
-        <v>0.70972222222222225</v>
+        <v>0.68472222222222223</v>
       </c>
       <c r="G207" s="37"/>
       <c r="H207" s="40" t="s">
@@ -10315,7 +10323,7 @@
     <row r="208" spans="1:8">
       <c r="A208" s="36" t="str">
         <f t="shared" si="4"/>
-        <v>Oceano_2015-06-03_BSNE_B2_1707_1737</v>
+        <v>Oceano_2015-06-03_BSNE_B2_1632_1702</v>
       </c>
       <c r="B208" s="42" t="s">
         <v>5</v>
@@ -10327,10 +10335,10 @@
         <v>10</v>
       </c>
       <c r="E208" s="41">
-        <v>0.71319444444444446</v>
+        <v>0.68888888888888899</v>
       </c>
       <c r="F208" s="41">
-        <v>0.73402777777777783</v>
+        <v>0.70972222222222225</v>
       </c>
       <c r="G208" s="37"/>
       <c r="H208" s="40" t="s">
@@ -10340,7 +10348,7 @@
     <row r="209" spans="1:8">
       <c r="A209" s="36" t="str">
         <f t="shared" si="4"/>
-        <v>Oceano_2015-06-03_BSNE_B2_1743_1813</v>
+        <v>Oceano_2015-06-03_BSNE_B2_1707_1737</v>
       </c>
       <c r="B209" s="42" t="s">
         <v>5</v>
@@ -10352,10 +10360,10 @@
         <v>10</v>
       </c>
       <c r="E209" s="41">
-        <v>0.73819444444444438</v>
+        <v>0.71319444444444446</v>
       </c>
       <c r="F209" s="41">
-        <v>0.75902777777777775</v>
+        <v>0.73402777777777783</v>
       </c>
       <c r="G209" s="37"/>
       <c r="H209" s="40" t="s">
@@ -10365,7 +10373,7 @@
     <row r="210" spans="1:8">
       <c r="A210" s="36" t="str">
         <f t="shared" si="4"/>
-        <v>Oceano_2015-06-03_BSNE_B3_1040_1813</v>
+        <v>Oceano_2015-06-03_BSNE_B2_1743_1813</v>
       </c>
       <c r="B210" s="42" t="s">
         <v>5</v>
@@ -10374,17 +10382,15 @@
         <v>42158</v>
       </c>
       <c r="D210" s="42" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E210" s="41">
-        <v>0.44444444444444442</v>
+        <v>0.73819444444444438</v>
       </c>
       <c r="F210" s="41">
         <v>0.75902777777777775</v>
       </c>
-      <c r="G210" s="37" t="s">
-        <v>31</v>
-      </c>
+      <c r="G210" s="37"/>
       <c r="H210" s="40" t="s">
         <v>29</v>
       </c>
@@ -10392,7 +10398,7 @@
     <row r="211" spans="1:8">
       <c r="A211" s="36" t="str">
         <f t="shared" si="4"/>
-        <v>Oceano_2015-06-03_BSNE_B4_1040_1345</v>
+        <v>Oceano_2015-06-03_BSNE_B3_1040_1813</v>
       </c>
       <c r="B211" s="42" t="s">
         <v>5</v>
@@ -10401,15 +10407,17 @@
         <v>42158</v>
       </c>
       <c r="D211" s="42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E211" s="41">
         <v>0.44444444444444442</v>
       </c>
       <c r="F211" s="41">
-        <v>0.57291666666666663</v>
-      </c>
-      <c r="G211" s="37"/>
+        <v>0.75902777777777775</v>
+      </c>
+      <c r="G211" s="37" t="s">
+        <v>31</v>
+      </c>
       <c r="H211" s="40" t="s">
         <v>29</v>
       </c>
@@ -10417,7 +10425,7 @@
     <row r="212" spans="1:8">
       <c r="A212" s="36" t="str">
         <f t="shared" si="4"/>
-        <v>Oceano_2015-06-03_BSNE_B4_1352_1437</v>
+        <v>Oceano_2015-06-03_BSNE_B4_1040_1345</v>
       </c>
       <c r="B212" s="42" t="s">
         <v>5</v>
@@ -10429,14 +10437,12 @@
         <v>17</v>
       </c>
       <c r="E212" s="41">
-        <v>0.57777777777777783</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="F212" s="41">
-        <v>0.60902777777777783</v>
-      </c>
-      <c r="G212" s="37" t="s">
-        <v>27</v>
-      </c>
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="G212" s="37"/>
       <c r="H212" s="40" t="s">
         <v>29</v>
       </c>
@@ -10444,7 +10450,7 @@
     <row r="213" spans="1:8">
       <c r="A213" s="36" t="str">
         <f t="shared" si="4"/>
-        <v>Oceano_2015-06-03_BSNE_B4_1444_1514</v>
+        <v>Oceano_2015-06-03_BSNE_B4_1352_1437</v>
       </c>
       <c r="B213" s="42" t="s">
         <v>5</v>
@@ -10456,10 +10462,10 @@
         <v>17</v>
       </c>
       <c r="E213" s="41">
-        <v>0.61388888888888882</v>
+        <v>0.57777777777777783</v>
       </c>
       <c r="F213" s="41">
-        <v>0.63472222222222219</v>
+        <v>0.60902777777777783</v>
       </c>
       <c r="G213" s="37" t="s">
         <v>27</v>
@@ -10471,7 +10477,7 @@
     <row r="214" spans="1:8">
       <c r="A214" s="36" t="str">
         <f t="shared" si="4"/>
-        <v>Oceano_2015-06-03_BSNE_B4_1520_1550</v>
+        <v>Oceano_2015-06-03_BSNE_B4_1444_1514</v>
       </c>
       <c r="B214" s="42" t="s">
         <v>5</v>
@@ -10483,10 +10489,10 @@
         <v>17</v>
       </c>
       <c r="E214" s="41">
-        <v>0.63888888888888895</v>
+        <v>0.61388888888888882</v>
       </c>
       <c r="F214" s="41">
-        <v>0.65972222222222221</v>
+        <v>0.63472222222222219</v>
       </c>
       <c r="G214" s="37" t="s">
         <v>27</v>
@@ -10498,7 +10504,7 @@
     <row r="215" spans="1:8">
       <c r="A215" s="36" t="str">
         <f t="shared" si="4"/>
-        <v>Oceano_2015-06-03_BSNE_B4_1556_1626</v>
+        <v>Oceano_2015-06-03_BSNE_B4_1520_1550</v>
       </c>
       <c r="B215" s="42" t="s">
         <v>5</v>
@@ -10510,12 +10516,14 @@
         <v>17</v>
       </c>
       <c r="E215" s="41">
-        <v>0.66388888888888886</v>
+        <v>0.63888888888888895</v>
       </c>
       <c r="F215" s="41">
-        <v>0.68472222222222223</v>
-      </c>
-      <c r="G215" s="37"/>
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="G215" s="37" t="s">
+        <v>27</v>
+      </c>
       <c r="H215" s="40" t="s">
         <v>29</v>
       </c>
@@ -10523,7 +10531,7 @@
     <row r="216" spans="1:8">
       <c r="A216" s="36" t="str">
         <f t="shared" si="4"/>
-        <v>Oceano_2015-06-03_BSNE_B4_1632_1702</v>
+        <v>Oceano_2015-06-03_BSNE_B4_1556_1626</v>
       </c>
       <c r="B216" s="42" t="s">
         <v>5</v>
@@ -10535,14 +10543,12 @@
         <v>17</v>
       </c>
       <c r="E216" s="41">
-        <v>0.68888888888888899</v>
+        <v>0.66388888888888886</v>
       </c>
       <c r="F216" s="41">
-        <v>0.70972222222222225</v>
-      </c>
-      <c r="G216" s="37" t="s">
-        <v>27</v>
-      </c>
+        <v>0.68472222222222223</v>
+      </c>
+      <c r="G216" s="37"/>
       <c r="H216" s="40" t="s">
         <v>29</v>
       </c>
@@ -10550,7 +10556,7 @@
     <row r="217" spans="1:8">
       <c r="A217" s="36" t="str">
         <f t="shared" si="4"/>
-        <v>Oceano_2015-06-03_BSNE_B4_1707_1737</v>
+        <v>Oceano_2015-06-03_BSNE_B4_1632_1702</v>
       </c>
       <c r="B217" s="42" t="s">
         <v>5</v>
@@ -10562,88 +10568,115 @@
         <v>17</v>
       </c>
       <c r="E217" s="41">
+        <v>0.68888888888888899</v>
+      </c>
+      <c r="F217" s="41">
+        <v>0.70972222222222225</v>
+      </c>
+      <c r="G217" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="H217" s="40" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8">
+      <c r="A218" s="36" t="str">
+        <f t="shared" si="4"/>
+        <v>Oceano_2015-06-03_BSNE_B4_1707_1737</v>
+      </c>
+      <c r="B218" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C218" s="38">
+        <v>42158</v>
+      </c>
+      <c r="D218" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="E218" s="41">
         <v>0.71319444444444446</v>
       </c>
-      <c r="F217" s="41">
+      <c r="F218" s="41">
         <v>0.73402777777777783</v>
       </c>
-      <c r="G217" s="37"/>
-      <c r="H217" s="40" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="218" spans="1:8">
-      <c r="A218" s="44" t="str">
+      <c r="G218" s="37"/>
+      <c r="H218" s="40" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8">
+      <c r="A219" s="44" t="str">
         <f t="shared" si="4"/>
         <v>Oceano_2015-06-03_BSNE_B4_1743_1813</v>
       </c>
-      <c r="B218" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="C218" s="46">
+      <c r="B219" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C219" s="46">
         <v>42158</v>
       </c>
-      <c r="D218" s="45" t="s">
+      <c r="D219" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="E218" s="47">
+      <c r="E219" s="47">
         <v>0.73819444444444438</v>
       </c>
-      <c r="F218" s="47">
+      <c r="F219" s="47">
         <v>0.75902777777777775</v>
       </c>
-      <c r="G218" s="48"/>
-      <c r="H218" s="49" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="219" spans="1:8">
-      <c r="A219" s="36" t="str">
+      <c r="G219" s="48"/>
+      <c r="H219" s="49" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8">
+      <c r="A220" s="36" t="str">
         <f t="shared" si="4"/>
         <v>Oceano_2015-06-04_BSNE_A3_1121_1500</v>
       </c>
-      <c r="B219" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="C219" s="38">
+      <c r="B220" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C220" s="38">
         <v>42159</v>
       </c>
-      <c r="D219" s="42" t="s">
+      <c r="D220" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="E219" s="41">
+      <c r="E220" s="41">
         <v>0.47291666666666665</v>
       </c>
-      <c r="F219" s="41">
+      <c r="F220" s="41">
         <v>0.625</v>
       </c>
-      <c r="G219" s="37"/>
-      <c r="H219" s="40" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="220" spans="1:8">
-      <c r="A220" s="44" t="str">
+      <c r="G220" s="37"/>
+      <c r="H220" s="40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8">
+      <c r="A221" s="44" t="str">
         <f t="shared" si="4"/>
         <v>Oceano_2015-06-04_BSNE_A4_1121_1500</v>
       </c>
-      <c r="B220" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="C220" s="46">
+      <c r="B221" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C221" s="46">
         <v>42159</v>
       </c>
-      <c r="D220" s="45" t="s">
+      <c r="D221" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="E220" s="47">
+      <c r="E221" s="47">
         <v>0.47291666666666665</v>
       </c>
-      <c r="F220" s="47">
+      <c r="F221" s="47">
         <v>0.625</v>
       </c>
-      <c r="G220" s="48"/>
-      <c r="H220" s="49" t="s">
+      <c r="G221" s="48"/>
+      <c r="H221" s="49" t="s">
         <v>30</v>
       </c>
     </row>
@@ -10661,10 +10694,10 @@
     <brk id="50" max="16383" man="1"/>
     <brk id="74" max="16383" man="1"/>
     <brk id="103" max="16383" man="1"/>
-    <brk id="130" max="16383" man="1"/>
-    <brk id="133" max="16383" man="1"/>
-    <brk id="173" max="16383" man="1"/>
-    <brk id="218" max="16383" man="1"/>
+    <brk id="131" max="16383" man="1"/>
+    <brk id="134" max="16383" man="1"/>
+    <brk id="174" max="16383" man="1"/>
+    <brk id="219" max="16383" man="1"/>
   </rowBreaks>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>